<commit_message>
Añadio compatibilidad con Ldap
</commit_message>
<xml_diff>
--- a/adminstrador-procesos/latinus-parent/documentos/Maquina de Estados - Tiempos y Alcance.xlsx
+++ b/adminstrador-procesos/latinus-parent/documentos/Maquina de Estados - Tiempos y Alcance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edison\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edison\Documents\GitHub\latinus-administrador-procesos\adminstrador-procesos\latinus-parent\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -548,7 +548,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
@@ -6890,6 +6890,848 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>188357</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="CuadroTexto 29"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1619251" y="2295525"/>
+          <a:ext cx="1104900" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="es-ES"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1200"/>
+            <a:t>Adminsitrador</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>7382</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="CuadroTexto 29"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2800350" y="2305050"/>
+          <a:ext cx="704850" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="es-ES"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1200"/>
+            <a:t>Juridico</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>150257</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="CuadroTexto 29"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4495799" y="352425"/>
+          <a:ext cx="1171575" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="es-ES"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1200"/>
+            <a:t>Administrador Registro Civil </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>131207</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="CuadroTexto 29"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4381500" y="3190875"/>
+          <a:ext cx="1104900" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="es-ES"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1200"/>
+            <a:t>Adminsitrador</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>121682</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="CuadroTexto 29"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6276975" y="2228850"/>
+          <a:ext cx="1104900" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="es-ES"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1200"/>
+            <a:t>Adminsitrador</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>695326</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>169307</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="CuadroTexto 29"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="352426" y="2276475"/>
+          <a:ext cx="1104900" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="es-ES"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1200"/>
+            <a:t>Administrador Registro Civil </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7793,7 +8635,7 @@
   <dimension ref="B2:AY27"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="K4" sqref="K4:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9868,8 +10710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>